<commit_message>
Added news to the header in all pages
</commit_message>
<xml_diff>
--- a/scope.XLSX
+++ b/scope.XLSX
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="209">
   <si>
     <t>ROOM</t>
   </si>
@@ -1265,9 +1265,9 @@
   <dimension ref="A1:O205"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78:XFD78"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1354,9 +1354,7 @@
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="B4"/>
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Added new page design principles
</commit_message>
<xml_diff>
--- a/scope.XLSX
+++ b/scope.XLSX
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\03_Website\_TIL Website\TIL with python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\03_Website\_TIL Website\TIL with python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$1:$206</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$1:$207</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="212">
   <si>
     <t>ROOM</t>
   </si>
@@ -656,6 +656,9 @@
   </si>
   <si>
     <t>fall/winter 2021</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1282,25 +1285,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O206"/>
+  <dimension ref="A1:O207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A151" sqref="A151"/>
+      <selection pane="bottomLeft" activeCell="G203" sqref="G203"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
     <col min="3" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="23" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -1324,7 +1327,7 @@
       </c>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +1416,7 @@
       </c>
       <c r="H5" s="27"/>
     </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1484,7 @@
       </c>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1505,7 +1508,7 @@
       </c>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
@@ -1527,7 +1530,7 @@
       </c>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -1547,7 +1550,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -1567,7 +1570,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -1591,7 +1594,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
@@ -1615,7 +1618,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
@@ -1684,7 +1687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>30</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>8</v>
       </c>
@@ -1864,7 +1867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>9</v>
       </c>
@@ -1888,7 +1891,7 @@
       </c>
       <c r="H26" s="25"/>
     </row>
-    <row r="27" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>10</v>
       </c>
@@ -1909,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>31</v>
       </c>
@@ -1928,7 +1931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>32</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1972,7 +1975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1993,7 +1996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>35</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>36</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>36</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>37</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>37</v>
       </c>
@@ -2082,7 +2085,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>38</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -2114,7 +2117,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>39</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>39</v>
       </c>
@@ -2146,7 +2149,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>40</v>
       </c>
@@ -2162,7 +2165,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>40</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>1</v>
       </c>
@@ -2202,7 +2205,7 @@
       </c>
       <c r="H43" s="27"/>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>3</v>
       </c>
@@ -2226,7 +2229,7 @@
       </c>
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>41</v>
       </c>
@@ -2242,7 +2245,7 @@
       </c>
       <c r="H45" s="23"/>
     </row>
-    <row r="46" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>42</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>43</v>
       </c>
@@ -2273,7 +2276,7 @@
       </c>
       <c r="H47" s="25"/>
     </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>44</v>
       </c>
@@ -2289,7 +2292,7 @@
       </c>
       <c r="H48" s="25"/>
     </row>
-    <row r="49" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>45</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>46</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>47</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>48</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>179</v>
       </c>
@@ -2378,7 +2381,7 @@
       <c r="F53" s="10"/>
       <c r="G53" s="29"/>
     </row>
-    <row r="54" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>49</v>
       </c>
@@ -2401,7 +2404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>180</v>
       </c>
@@ -2414,7 +2417,7 @@
       <c r="F55" s="10"/>
       <c r="G55" s="29"/>
     </row>
-    <row r="56" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>50</v>
       </c>
@@ -2431,7 +2434,7 @@
       <c r="F56"/>
       <c r="G56"/>
     </row>
-    <row r="57" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>51</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>51</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>52</v>
       </c>
@@ -2481,7 +2484,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>52</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>53</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>54</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>54</v>
       </c>
@@ -2549,7 +2552,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>55</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>55</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>197</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>56</v>
       </c>
@@ -2614,7 +2617,7 @@
       </c>
       <c r="G67" s="12"/>
     </row>
-    <row r="68" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>57</v>
       </c>
@@ -2634,7 +2637,7 @@
       </c>
       <c r="H68" s="25"/>
     </row>
-    <row r="69" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>58</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>59</v>
       </c>
@@ -2672,7 +2675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>198</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>60</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>204</v>
       </c>
@@ -2720,7 +2723,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>194</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>61</v>
       </c>
@@ -2758,7 +2761,7 @@
       </c>
       <c r="H75" s="27"/>
     </row>
-    <row r="76" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>62</v>
       </c>
@@ -2777,73 +2780,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>203</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D77" s="46"/>
-      <c r="E77" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F77" s="8" t="s">
+      <c r="C77"/>
+      <c r="D77" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B78"/>
+      <c r="C78" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="46"/>
+      <c r="E78" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="G77" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H77" s="23" t="s">
+      <c r="G78" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H78" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="7" t="s">
+    <row r="79" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="7" t="s">
+      <c r="B79" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F79" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G79" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>4</v>
@@ -2860,9 +2860,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>4</v>
@@ -2879,9 +2879,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>4</v>
@@ -2898,71 +2898,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F83" s="8" t="s">
+      <c r="B84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="G83" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="7" t="s">
+      <c r="G84" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C84" s="6"/>
-      <c r="D84" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="20" t="s">
+      <c r="B85" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="B85" s="29"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E85" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="F85" s="29"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="23">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="20" t="s">
-        <v>182</v>
       </c>
       <c r="B86" s="29"/>
       <c r="C86" s="6"/>
@@ -2978,221 +2979,221 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="7" t="s">
+    <row r="87" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B87" s="29"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="23">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B87" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G87" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="7" t="s">
+      <c r="B88" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F88" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B88" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F88" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="7" t="s">
+      <c r="B89" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B89" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F89" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G89" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="7" t="s">
+      <c r="B90" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B90" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D90" s="6"/>
-      <c r="E90" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F90" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G90" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="7" t="s">
+      <c r="B91" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="6"/>
+      <c r="E91" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="7" t="s">
+      <c r="B92" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F92" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="7" t="s">
+      <c r="B93" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B93" s="29"/>
-      <c r="C93" s="6"/>
-      <c r="D93"/>
-      <c r="E93" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F93" s="29"/>
-      <c r="G93" s="29"/>
-      <c r="H93" s="23">
+      <c r="B94" s="29"/>
+      <c r="C94" s="6"/>
+      <c r="D94"/>
+      <c r="E94" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="23">
         <v>2017</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="7" t="s">
+    <row r="95" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F94" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G94" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="7" t="s">
+      <c r="B95" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F95" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B95" s="29"/>
-      <c r="C95" s="29"/>
-      <c r="D95"/>
-      <c r="E95" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F95" s="29"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="23">
+      <c r="B96" s="29"/>
+      <c r="C96" s="29"/>
+      <c r="D96"/>
+      <c r="E96" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="23">
         <v>2017</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="7" t="s">
+    <row r="97" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B96" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F96" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G96" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="20" t="s">
+      <c r="B97" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="20" t="s">
         <v>184</v>
-      </c>
-      <c r="B97" s="29"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E97" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="F97" s="29"/>
-      <c r="G97" s="29"/>
-      <c r="H97" s="23">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="20" t="s">
-        <v>183</v>
       </c>
       <c r="B98" s="29"/>
       <c r="C98" s="29"/>
@@ -3208,9 +3209,9 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="20" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="B99" s="29"/>
       <c r="C99" s="29"/>
@@ -3223,31 +3224,30 @@
       <c r="F99" s="29"/>
       <c r="G99" s="29"/>
       <c r="H99" s="23">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F100" s="29"/>
+      <c r="G100" s="29"/>
+      <c r="H100" s="23">
         <v>2016</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="7" t="s">
+    <row r="101" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F100" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G100" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>4</v>
@@ -3264,9 +3264,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>4</v>
@@ -3283,9 +3283,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>4</v>
@@ -3301,11 +3301,10 @@
       <c r="G103" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H103" s="23"/>
-    </row>
-    <row r="104" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>4</v>
@@ -3323,9 +3322,9 @@
       </c>
       <c r="H104" s="23"/>
     </row>
-    <row r="105" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>4</v>
@@ -3341,10 +3340,11 @@
       <c r="G105" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H105" s="23"/>
+    </row>
+    <row r="106" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>4</v>
@@ -3361,27 +3361,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="20" t="s">
+    <row r="107" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="20" t="s">
         <v>185</v>
-      </c>
-      <c r="B107" s="29"/>
-      <c r="C107" s="6"/>
-      <c r="D107" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E107" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="23">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="20" t="s">
-        <v>186</v>
       </c>
       <c r="B108" s="29"/>
       <c r="C108" s="6"/>
@@ -3393,13 +3394,13 @@
       </c>
       <c r="F108" s="29"/>
       <c r="G108" s="29"/>
-      <c r="H108" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H108" s="23">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B109" s="29"/>
       <c r="C109" s="6"/>
@@ -3415,9 +3416,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B110" s="29"/>
       <c r="C110" s="6"/>
@@ -3429,33 +3430,31 @@
       </c>
       <c r="F110" s="29"/>
       <c r="G110" s="29"/>
-      <c r="H110" s="23">
+      <c r="H110" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B111" s="29"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E111" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F111" s="29"/>
+      <c r="G111" s="29"/>
+      <c r="H111" s="23">
         <v>2017</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="7" t="s">
+    <row r="112" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F111" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G111" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H111" s="23"/>
-    </row>
-    <row r="112" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>4</v>
@@ -3473,9 +3472,9 @@
       </c>
       <c r="H112" s="23"/>
     </row>
-    <row r="113" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>4</v>
@@ -3491,10 +3490,11 @@
       <c r="G113" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H113" s="23"/>
+    </row>
+    <row r="114" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>4</v>
@@ -3511,16 +3511,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="C115" s="6"/>
       <c r="D115" s="6"/>
       <c r="E115" s="8" t="s">
         <v>4</v>
@@ -3532,9 +3530,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>4</v>
@@ -3553,121 +3551,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117" s="6"/>
+      <c r="E117" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B117" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F117" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G117" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H117" s="23"/>
-    </row>
-    <row r="118" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="7" t="s">
+      <c r="B118" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F118" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H118" s="23"/>
+    </row>
+    <row r="119" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B118" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C118" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D118" s="10"/>
-      <c r="E118" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F118" s="8" t="s">
+      <c r="B119" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119" s="10"/>
+      <c r="E119" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F119" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="G118" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H118" s="23"/>
-    </row>
-    <row r="119" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="7" t="s">
+      <c r="G119" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H119" s="23"/>
+    </row>
+    <row r="120" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F119" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G119" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H119" s="23"/>
-    </row>
-    <row r="120" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="7" t="s">
+      <c r="B120" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E120" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G120" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H120" s="23"/>
+    </row>
+    <row r="121" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B120" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F120" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G120" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H120" s="25"/>
-    </row>
-    <row r="121" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="7" t="s">
+      <c r="B121" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H121" s="25"/>
+    </row>
+    <row r="122" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C121" s="6"/>
-      <c r="D121" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E121" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F121" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G121" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H121" s="23"/>
-    </row>
-    <row r="122" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>4</v>
@@ -3685,43 +3682,47 @@
       <c r="G122" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H122" s="23"/>
+    </row>
+    <row r="123" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123" s="6"/>
+      <c r="D123" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F123" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B123"/>
-      <c r="C123" s="6"/>
-      <c r="D123" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E123" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="F123" s="29"/>
-      <c r="G123" s="29"/>
-    </row>
-    <row r="124" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B124" s="29"/>
-      <c r="C124" s="29"/>
-      <c r="D124" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E124" s="21" t="s">
+      <c r="B124"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E124" s="47" t="s">
         <v>4</v>
       </c>
       <c r="F124" s="29"/>
       <c r="G124" s="29"/>
-      <c r="H124" s="23">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:8" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B125" s="29"/>
       <c r="C125" s="29"/>
@@ -3737,9 +3738,9 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B126" s="29"/>
       <c r="C126" s="29"/>
@@ -3755,121 +3756,116 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B127" s="29"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E127" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F127" s="29"/>
+      <c r="G127" s="29"/>
+      <c r="H127" s="23">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B127" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C127" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E127" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F127" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G127" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="7" t="s">
+      <c r="B128" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E128" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F128" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G128" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B128" s="29"/>
-      <c r="C128" s="29"/>
-      <c r="D128" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F128" s="29"/>
-      <c r="G128" s="29"/>
-      <c r="H128" s="23">
+      <c r="B129" s="29"/>
+      <c r="C129" s="29"/>
+      <c r="D129" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E129" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F129" s="29"/>
+      <c r="G129" s="29"/>
+      <c r="H129" s="23">
         <v>2017</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="7" t="s">
+    <row r="130" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B129" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D129" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E129" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F129" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G129" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="7" t="s">
+      <c r="B130" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F130" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G130" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B130" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C130" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D130" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E130" s="6"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="16" t="s">
+      <c r="B131" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B131" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C131" s="13"/>
-      <c r="D131" s="13"/>
-      <c r="E131" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F131" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="G131" s="18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="16" t="s">
-        <v>101</v>
-      </c>
       <c r="B132" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C132" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D132" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
       <c r="E132" s="17" t="s">
         <v>4</v>
       </c>
@@ -3880,173 +3876,175 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="7" t="s">
+    <row r="133" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B133" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C133" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D133" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E133" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F133" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="G133" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B133" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C133" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D133" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F133" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G133" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="7" t="s">
+      <c r="B134" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E134" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F134" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G134" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B134" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C134" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D134" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E134" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F134" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G134" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H134" s="27"/>
-    </row>
-    <row r="135" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="7" t="s">
+      <c r="B135" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D135" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E135" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F135" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G135" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H135" s="27"/>
+    </row>
+    <row r="136" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B135" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C135" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D135" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E135" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F135" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G135" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="7" t="s">
+      <c r="B136" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D136" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E136" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F136" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G136" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B136" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C136" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D136" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E136" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F136" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G136" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="7" t="s">
+      <c r="B137" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F137" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G137" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B137" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D137" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E137" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F137" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G137" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="7" t="s">
+      <c r="B138" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E138" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F138" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G138" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B138" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C138" s="6"/>
-      <c r="D138" s="6"/>
-      <c r="E138" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F138" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G138" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="16" t="s">
+      <c r="B139" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F139" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G139" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B139" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C139" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D139" s="9"/>
-      <c r="E139" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F139" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="G139" s="18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="16" t="s">
-        <v>109</v>
-      </c>
       <c r="B140" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C140" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D140" s="13"/>
+      <c r="D140" s="9"/>
       <c r="E140" s="17" t="s">
         <v>4</v>
       </c>
@@ -4056,146 +4054,146 @@
       <c r="G140" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H140" s="27"/>
-    </row>
-    <row r="141" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="7" t="s">
+    </row>
+    <row r="141" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B141" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C141" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D141" s="13"/>
+      <c r="E141" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F141" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="G141" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H141" s="27"/>
+    </row>
+    <row r="142" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B141" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C141" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D141" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E141" s="6"/>
-      <c r="F141" s="6"/>
-      <c r="G141" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="7" t="s">
+      <c r="B142" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B142" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C142" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D142" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E142" s="6"/>
-      <c r="F142" s="28"/>
-      <c r="G142" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="7" t="s">
+      <c r="B143" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D143" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E143" s="6"/>
+      <c r="F143" s="28"/>
+      <c r="G143" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B143" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D143" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E143" s="6"/>
-      <c r="F143" s="6"/>
-      <c r="G143" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="7" t="s">
+      <c r="B144" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B144" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C144" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D144" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E144" s="28"/>
-      <c r="F144" s="28"/>
-      <c r="G144" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B145"/>
-      <c r="C145"/>
-      <c r="D145"/>
+      <c r="B145" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D145" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="E145" s="28"/>
       <c r="F145" s="28"/>
       <c r="G145" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B146"/>
+      <c r="C146"/>
+      <c r="D146"/>
+      <c r="E146" s="28"/>
+      <c r="F146" s="28"/>
+      <c r="G146" s="38" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="16" t="s">
+    <row r="147" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B146" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C146" s="13"/>
-      <c r="D146" s="13"/>
-      <c r="E146" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F146" s="17" t="s">
+      <c r="B147" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F147" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="G146" s="18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="16" t="s">
+      <c r="G147" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B147" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C147" s="32"/>
-      <c r="D147" s="41"/>
-      <c r="E147" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F147" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="G147" s="39" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="B148" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C148" s="32"/>
-      <c r="D148" s="36" t="s">
-        <v>4</v>
-      </c>
+      <c r="D148" s="41"/>
       <c r="E148" s="36" t="s">
         <v>4</v>
       </c>
@@ -4206,38 +4204,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B149" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" s="32"/>
+      <c r="D149" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E149" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F149" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="G149" s="39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B149" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C149" s="13"/>
-      <c r="D149" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E149" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F149" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="G149" s="18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="16" t="s">
-        <v>118</v>
-      </c>
       <c r="B150" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C150" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D150" s="13"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="E150" s="17" t="s">
         <v>4</v>
       </c>
@@ -4248,96 +4246,98 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B151" s="10"/>
-      <c r="C151" s="9"/>
-      <c r="D151" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E151"/>
-      <c r="F151"/>
-      <c r="G151"/>
-      <c r="H151" s="23" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B151" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C151" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D151" s="13"/>
+      <c r="E151" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F151" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="G151" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B152" s="10"/>
       <c r="C152" s="9"/>
-      <c r="D152" s="11"/>
-      <c r="E152" s="30"/>
+      <c r="D152" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E152"/>
       <c r="F152"/>
       <c r="G152"/>
       <c r="H152" s="23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B153" s="10"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="11"/>
+      <c r="E153" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="F153"/>
+      <c r="G153"/>
+      <c r="H153" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="7" t="s">
+    <row r="154" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B153" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C153" s="6"/>
-      <c r="D153" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E153" s="6"/>
-      <c r="F153" s="6"/>
-      <c r="G153" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="7" t="s">
+      <c r="B154" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154" s="6"/>
+      <c r="D154" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B154" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C154" s="6"/>
-      <c r="D154" s="6"/>
-      <c r="E154" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F154" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G154" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="7" t="s">
+      <c r="B155" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F155" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G155" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="B155" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C155" s="6"/>
-      <c r="D155" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E155" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F155" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G155" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>4</v>
@@ -4356,53 +4356,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C157" s="6"/>
+      <c r="D157" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E157" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F157" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G157" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B157" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C157" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D157" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E157" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F157" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G157" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="7" t="s">
+      <c r="B158" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D158" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E158" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F158" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G158" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="B158" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C158" s="6"/>
-      <c r="D158" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E158" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F158" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G158" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="B159" s="22" t="s">
         <v>4</v>
@@ -4421,631 +4421,630 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B160" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C160" s="6"/>
+      <c r="D160" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E160" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F160" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G160" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B160" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C160" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D160" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E160" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F160" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G160" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="7" t="s">
+      <c r="B161" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C161" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D161" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E161" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F161" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G161" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E161" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F161" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G161" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="7" t="s">
+      <c r="B162" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F162" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G162" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B162" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C162" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D162" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E162" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F162" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G162" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="7" t="s">
+      <c r="B163" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D163" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E163" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F163" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G163" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B163" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C163" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D163" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E163" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F163" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G163" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="7" t="s">
+      <c r="B164" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D164" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E164" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F164" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G164" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B164" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C164" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E164" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F164" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G164" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="7" t="s">
+      <c r="B165" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D165" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E165" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F165" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G165" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B165" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C165" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D165" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E165" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F165" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G165" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="7" t="s">
+      <c r="B166" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D166" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E166" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F166" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G166" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B166" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C166" s="10"/>
-      <c r="D166" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E166" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F166" s="10"/>
-      <c r="G166"/>
-      <c r="H166" s="23">
+      <c r="B167" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C167" s="10"/>
+      <c r="D167" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E167" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F167" s="10"/>
+      <c r="G167"/>
+      <c r="H167" s="23">
         <v>2018</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="7" t="s">
+    <row r="168" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B167" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C167" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D167" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E167" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F167" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G167" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="7" t="s">
+      <c r="B168" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C168" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D168" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E168" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F168" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G168" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B168" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C168" s="6"/>
-      <c r="D168" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E168" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F168" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G168" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="7" t="s">
+      <c r="B169" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C169" s="6"/>
+      <c r="D169" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E169" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F169" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G169" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B169" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C169" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D169" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E169" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F169" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G169" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="7" t="s">
+      <c r="B170" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D170" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E170" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F170" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G170" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B170" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C170" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D170" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E170" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F170" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G170" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="7" t="s">
+      <c r="B171" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D171" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E171" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F171" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G171" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B171" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C171" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D171" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E171" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F171" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G171" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="7" t="s">
+      <c r="B172" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D172" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E172" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F172" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G172" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B172" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C172" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D172" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E172" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F172" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G172" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="7" t="s">
+      <c r="B173" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D173" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E173" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F173" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G173" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B173" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D173" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E173" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F173" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G173" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="7" t="s">
+      <c r="B174" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D174" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E174" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F174" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G174" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B174" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C174" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D174" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E174" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F174" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G174" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H174" s="25"/>
-    </row>
-    <row r="175" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="7" t="s">
+      <c r="B175" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C175" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E175" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F175" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G175" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H175" s="25"/>
+    </row>
+    <row r="176" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B175" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C175" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D175" s="6"/>
-      <c r="E175" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F175" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G175" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="7" t="s">
+      <c r="B176" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D176" s="6"/>
+      <c r="E176" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F176" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G176" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B176" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C176" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D176" s="34"/>
-      <c r="E176" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F176" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G176" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="7" t="s">
+      <c r="B177" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D177" s="34"/>
+      <c r="E177" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F177" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G177" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B177" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C177" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D177" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E177" s="6"/>
-      <c r="F177" s="6"/>
-      <c r="G177" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="7" t="s">
+      <c r="B178" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
+      <c r="G178" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B178" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C178" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D178" s="6"/>
-      <c r="E178" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F178" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G178" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="7" t="s">
+      <c r="B179" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D179" s="6"/>
+      <c r="E179" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F179" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G179" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B179" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C179" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D179" s="34"/>
-      <c r="E179" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F179" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G179" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="7" t="s">
+      <c r="B180" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C180" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D180" s="34"/>
+      <c r="E180" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F180" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G180" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B180" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C180" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D180" s="28"/>
-      <c r="E180" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F180" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G180" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="7" t="s">
+      <c r="B181" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D181" s="28"/>
+      <c r="E181" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F181" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G181" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B181" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C181" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D181" s="6"/>
-      <c r="E181" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F181" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G181" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="7" t="s">
+      <c r="B182" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D182" s="6"/>
+      <c r="E182" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F182" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G182" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B182" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C182" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D182" s="6"/>
-      <c r="E182" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F182" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G182" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="7" t="s">
+      <c r="B183" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C183" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D183" s="6"/>
+      <c r="E183" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F183" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G183" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B183" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C183" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D183" s="6"/>
-      <c r="E183" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F183" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G183" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184" s="7" t="s">
+      <c r="B184" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D184" s="6"/>
+      <c r="E184" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F184" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G184" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B184" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D184" s="6"/>
-      <c r="E184" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F184" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G184" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="7" t="s">
+      <c r="B185" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D185" s="6"/>
+      <c r="E185" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F185" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G185" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B185" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C185" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D185" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E185" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F185" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G185" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="7" t="s">
+      <c r="B186" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C186" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D186" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E186" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F186" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G186" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B186" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C186" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D186" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E186" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F186" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G186" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" s="7" t="s">
+      <c r="B187" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C187" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D187" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E187" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F187" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G187" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B187" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C187" s="6"/>
-      <c r="D187" s="6"/>
-      <c r="E187" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F187" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G187" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H187" s="25"/>
-    </row>
-    <row r="188" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="7" t="s">
-        <v>155</v>
-      </c>
       <c r="B188" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C188" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="C188" s="6"/>
       <c r="D188" s="6"/>
       <c r="E188" s="8" t="s">
         <v>4</v>
@@ -5053,13 +5052,14 @@
       <c r="F188" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G188" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G188" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H188" s="25"/>
+    </row>
+    <row r="189" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B189" s="8" t="s">
         <v>4</v>
@@ -5078,51 +5078,53 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D190" s="6"/>
+      <c r="E190" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F190" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G190" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B190" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C190" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D190" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E190" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F190" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G190" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" s="7" t="s">
+      <c r="B191" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D191" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F191" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G191" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="B191" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C191" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D191" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E191" s="6"/>
-      <c r="F191" s="6"/>
-      <c r="G191" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="B192" s="8" t="s">
         <v>4</v>
@@ -5139,28 +5141,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D193" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E193" s="6"/>
+      <c r="F193" s="6"/>
+      <c r="G193" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="B193" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F193" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G193" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A194" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="B194" s="8" t="s">
         <v>4</v>
@@ -5177,9 +5179,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B195" s="8" t="s">
         <v>4</v>
@@ -5196,16 +5198,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B196" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C196" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="C196" s="6"/>
       <c r="D196" s="6"/>
       <c r="E196" s="8" t="s">
         <v>4</v>
@@ -5217,138 +5217,132 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B197"/>
-      <c r="C197" s="6"/>
-      <c r="D197" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E197"/>
-      <c r="F197"/>
-      <c r="G197"/>
-      <c r="H197" s="23">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="198" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D197" s="6"/>
+      <c r="E197" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F197" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G197" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B198" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="B198"/>
       <c r="C198" s="6"/>
-      <c r="D198" s="10"/>
-      <c r="E198" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F198" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G198" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H198" s="23" t="s">
+      <c r="D198" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E198"/>
+      <c r="F198"/>
+      <c r="G198"/>
+      <c r="H198" s="23">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C199" s="6"/>
+      <c r="D199" s="10"/>
+      <c r="E199" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F199" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G199" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H199" s="23" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B199"/>
-      <c r="C199"/>
-      <c r="D199" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E199"/>
-      <c r="F199" s="6"/>
-      <c r="G199"/>
-      <c r="H199" s="23">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="200" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B200" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C200" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D200" s="10"/>
-      <c r="E200" s="6"/>
+      <c r="B200"/>
+      <c r="C200"/>
+      <c r="D200" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E200"/>
       <c r="F200" s="6"/>
-      <c r="G200" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H200" s="23" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="201" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G200"/>
+      <c r="H200" s="23">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B201"/>
       <c r="C201"/>
-      <c r="D201" s="40" t="s">
+      <c r="D201" s="10"/>
+      <c r="E201" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E201"/>
-      <c r="F201" s="28"/>
+      <c r="F201" s="6"/>
       <c r="G201"/>
-      <c r="H201" s="25">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="202" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H201" s="23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B202" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C202" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D202" s="31"/>
-      <c r="E202" s="28"/>
+      <c r="B202"/>
+      <c r="C202"/>
+      <c r="D202" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="E202"/>
       <c r="F202" s="28"/>
-      <c r="G202" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H202" s="23" t="s">
+      <c r="G202"/>
+      <c r="H202" s="25">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B203"/>
+      <c r="C203"/>
+      <c r="D203" s="31"/>
+      <c r="E203" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="F203" s="28"/>
+      <c r="G203"/>
+      <c r="H203" s="23" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="7" t="s">
+    <row r="204" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="B203" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C203" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D203" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E203" s="28"/>
-      <c r="F203" s="28"/>
-      <c r="G203" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="204" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="B204" s="22" t="s">
         <v>4</v>
@@ -5364,48 +5358,67 @@
       <c r="G204" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H204" s="25"/>
-    </row>
-    <row r="205" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="205" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B205" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D205" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E205" s="28"/>
+      <c r="F205" s="28"/>
+      <c r="G205" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H205" s="25"/>
+    </row>
+    <row r="206" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B205" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C205" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D205" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E205" s="28"/>
-      <c r="F205" s="6"/>
-      <c r="G205" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H205" s="26"/>
-    </row>
-    <row r="206" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A206" s="7" t="s">
+      <c r="B206" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C206" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D206" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E206" s="28"/>
+      <c r="F206" s="6"/>
+      <c r="G206" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H206" s="26"/>
+    </row>
+    <row r="207" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B206" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C206" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D206" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E206" s="6"/>
-      <c r="F206" s="6"/>
-      <c r="G206" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H206" s="27"/>
-      <c r="O206" s="23"/>
+      <c r="B207" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C207" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D207" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E207" s="6"/>
+      <c r="F207" s="6"/>
+      <c r="G207" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H207" s="27"/>
+      <c r="O207" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A5:I208">

</xml_diff>